<commit_message>
Analyse van Astrid verwerkt
</commit_message>
<xml_diff>
--- a/maps/MedicationStatement-Medicatieoverzicht.xlsx
+++ b/maps/MedicationStatement-Medicatieoverzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/jacob_engel_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{C7E22464-8063-5A48-8AF8-B8CBF9685F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01744243-E4FE-024B-9C89-9B514398D39A}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{C7E22464-8063-5A48-8AF8-B8CBF9685F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D45A7D0-CD62-B74D-B288-D5CCA6640D23}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="4140" windowWidth="22880" windowHeight="20140" xr2:uid="{4D4295CA-5E27-D54A-800A-CCB7595BF199}"/>
+    <workbookView xWindow="1860" yWindow="4620" windowWidth="22880" windowHeight="20140" xr2:uid="{4D4295CA-5E27-D54A-800A-CCB7595BF199}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>xtehr</t>
   </si>
@@ -96,81 +96,6 @@
   </si>
   <si>
     <t>EHDSMedicationStatement.periodOfUse</t>
-  </si>
-  <si>
-    <t>MedicationAgreement</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.PrescriptionReason</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.PrescriptionReason.Diagnosis</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.PrescriptionReason.HypersensitivityIntolerance</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.PrescriptionReason.Reaction</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.PrescriptionReason.Symptom</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.Prescriber::HealthProfessional</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.AgreedMedicine::PharmaceuticalProduct</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.InstructionsForUse</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.MedicationAgreementDateTime</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.PeriodOfUse::TimeInterval</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.MedicationAgreementStopType</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.ReasonModificationOrDiscontinuation</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.MedicationAgreementAdditionalInformation</t>
-  </si>
-  <si>
-    <t>MedicationAgreement.Comment</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.AdministrationAgreementReasonModificationOrDiscontinuation</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.Supplier::HealthcareProvider</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.MedicineForAdministrationAgreement::PharmaceuticalProduct</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.InstructionsForUse</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.AdministrationAgreementDateTime</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.PeriodOfUse</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.MedicationAgreement</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.AdministrationAgreementStopType</t>
-  </si>
-  <si>
-    <t>AdministrationAgreement.Comment</t>
   </si>
   <si>
     <t>MedicationUse</t>
@@ -609,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81200B0-CEC8-5048-84D0-94AD3B33B9B6}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,6 +558,9 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -688,11 +616,17 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -703,6 +637,9 @@
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -713,195 +650,46 @@
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>22</v>
+      <c r="B22" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>23</v>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>24</v>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+      <c r="B25" s="2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -910,6 +698,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
+    <Inhoud xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAFAE49EF5FC2A44A9A24B379C77993A" ma:contentTypeVersion="18" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4e3f09d53704208a567efd423a8e8ffb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b19602bd-a67a-4df8-b412-b401dd608f7a" xmlns:ns3="3af30693-c405-4a5b-908a-bd1dc294f76b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e8dd9eed0ce6952e5fe39cbc0c50bd" ns2:_="" ns3:_="">
     <xsd:import namespace="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
@@ -1166,28 +975,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
-    <Inhoud xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E843A67A-5CFA-4676-B15B-2998016625A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970B705-F7BE-41C9-8DD2-E2B6E519E36A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3af30693-c405-4a5b-908a-bd1dc294f76b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E095BA-029E-4CD0-B562-1B5D059A55A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1204,29 +1017,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970B705-F7BE-41C9-8DD2-E2B6E519E36A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3af30693-c405-4a5b-908a-bd1dc294f76b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E843A67A-5CFA-4676-B15B-2998016625A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>